<commit_message>
Enhanced Shift Handover Application with SSO Integration
 Major Features Added:
- Multi-provider SSO authentication (Google OAuth, Azure AD, SAML, LDAP)
- Admin SSO configuration dashboard and management interface
- Encrypted SSO provider configuration storage
- Role-based access control for SSO settings
- Enhanced navigation with SSO Configuration tab

 Core Improvements:
- Database models for SSO configuration with encryption
- OAuth 2.0 authentication flows and user provisioning
- ServiceNow integration for automated CTask assignment
- Enhanced dashboard with modern UI components
- Comprehensive audit logging and security features

 New Components:
- SSO authentication routes and configuration management
- Admin templates for SSO dashboard and provider setup
- Database migrations for new SSO tables
- Production deployment configurations
- Security enhancements and error handling

 Ready for Azure DevOps deployment with complete SSO functionality
</commit_message>
<xml_diff>
--- a/uploads/roster/acme_corp_team_a_roster.xlsx
+++ b/uploads/roster/acme_corp_team_a_roster.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SajidMohammad\Downloads\sh tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://epam-my.sharepoint.com/personal/sajid_mohammad_epam_com/Documents/Shift Handover App/sh tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8943C1-D3CA-4082-969B-F66C8D01F254}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{5C4ED353-8791-4525-B3F1-D72250515BCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2EBBFD0-A3AB-4DEC-8A7C-95C07D91B8FF}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{5E123F2D-510B-42EA-A8E2-E3780960F3A0}"/>
+    <workbookView xWindow="-28920" yWindow="1605" windowWidth="29040" windowHeight="15720" xr2:uid="{5E123F2D-510B-42EA-A8E2-E3780960F3A0}"/>
   </bookViews>
   <sheets>
     <sheet name="acme_corp_team_a" sheetId="1" r:id="rId1"/>
@@ -663,8 +663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9976DB49-D0ED-4D1D-BE76-DE8DCCD75B0B}">
   <dimension ref="A1:AF12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="X4" sqref="X4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -678,97 +678,97 @@
         <v>25</v>
       </c>
       <c r="B1" s="1">
-        <v>45870</v>
+        <v>45931</v>
       </c>
       <c r="C1" s="1">
-        <v>45871</v>
+        <v>45932</v>
       </c>
       <c r="D1" s="1">
-        <v>45872</v>
+        <v>45933</v>
       </c>
       <c r="E1" s="1">
-        <v>45873</v>
+        <v>45934</v>
       </c>
       <c r="F1" s="1">
-        <v>45874</v>
+        <v>45935</v>
       </c>
       <c r="G1" s="1">
-        <v>45875</v>
+        <v>45936</v>
       </c>
       <c r="H1" s="1">
-        <v>45876</v>
+        <v>45937</v>
       </c>
       <c r="I1" s="1">
-        <v>45877</v>
+        <v>45938</v>
       </c>
       <c r="J1" s="1">
-        <v>45878</v>
+        <v>45939</v>
       </c>
       <c r="K1" s="1">
-        <v>45879</v>
+        <v>45940</v>
       </c>
       <c r="L1" s="1">
-        <v>45880</v>
+        <v>45941</v>
       </c>
       <c r="M1" s="1">
-        <v>45881</v>
+        <v>45942</v>
       </c>
       <c r="N1" s="1">
-        <v>45882</v>
+        <v>45943</v>
       </c>
       <c r="O1" s="1">
-        <v>45883</v>
+        <v>45944</v>
       </c>
       <c r="P1" s="1">
-        <v>45884</v>
+        <v>45945</v>
       </c>
       <c r="Q1" s="1">
-        <v>45885</v>
+        <v>45946</v>
       </c>
       <c r="R1" s="1">
-        <v>45886</v>
+        <v>45947</v>
       </c>
       <c r="S1" s="1">
-        <v>45887</v>
+        <v>45948</v>
       </c>
       <c r="T1" s="1">
-        <v>45888</v>
+        <v>45949</v>
       </c>
       <c r="U1" s="1">
-        <v>45889</v>
+        <v>45950</v>
       </c>
       <c r="V1" s="1">
-        <v>45890</v>
+        <v>45951</v>
       </c>
       <c r="W1" s="1">
-        <v>45891</v>
+        <v>45952</v>
       </c>
       <c r="X1" s="1">
-        <v>45892</v>
+        <v>45953</v>
       </c>
       <c r="Y1" s="1">
-        <v>45893</v>
+        <v>45954</v>
       </c>
       <c r="Z1" s="1">
-        <v>45894</v>
+        <v>45955</v>
       </c>
       <c r="AA1" s="1">
-        <v>45895</v>
+        <v>45956</v>
       </c>
       <c r="AB1" s="1">
-        <v>45896</v>
+        <v>45957</v>
       </c>
       <c r="AC1" s="1">
-        <v>45897</v>
+        <v>45958</v>
       </c>
       <c r="AD1" s="1">
-        <v>45898</v>
+        <v>45959</v>
       </c>
       <c r="AE1" s="1">
-        <v>45899</v>
+        <v>45960</v>
       </c>
       <c r="AF1" s="1">
-        <v>45900</v>
+        <v>45961</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.3">

</xml_diff>